<commit_message>
Web Scraping NBA Awards
</commit_message>
<xml_diff>
--- a/resources/nba_results.xlsx
+++ b/resources/nba_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clewe\ETL_project\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D000C07-3E47-4511-A4B4-0E79AAEBCB5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06123DCB-2CB6-4F3A-BABF-B31941035D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E9BA98B-B04A-4286-9670-24D44481C6C6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="545">
   <si>
     <t>Season</t>
   </si>
@@ -1004,24 +1004,6 @@
     <t>WS</t>
   </si>
   <si>
-    <t>MVP_player_page</t>
-  </si>
-  <si>
-    <t>ROY_player_page</t>
-  </si>
-  <si>
-    <t>PTS_player_page</t>
-  </si>
-  <si>
-    <t>TRB_player_page</t>
-  </si>
-  <si>
-    <t>AST_player_page</t>
-  </si>
-  <si>
-    <t>WS_player_page</t>
-  </si>
-  <si>
     <t>2019-20</t>
   </si>
   <si>
@@ -1062,6 +1044,630 @@
   </si>
   <si>
     <t>J. Harden (15.2)</t>
+  </si>
+  <si>
+    <t>ABA</t>
+  </si>
+  <si>
+    <t>New York Nets</t>
+  </si>
+  <si>
+    <t>D. Thompson</t>
+  </si>
+  <si>
+    <t>J. Erving (2462)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (1303)</t>
+  </si>
+  <si>
+    <t>D. Buse (689)</t>
+  </si>
+  <si>
+    <t>J. Erving (17.7)</t>
+  </si>
+  <si>
+    <t>Kentucky Colonels</t>
+  </si>
+  <si>
+    <t>M. Barnes</t>
+  </si>
+  <si>
+    <t>G. McGinnis (2353)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (1361)</t>
+  </si>
+  <si>
+    <t>C. Williams (576)</t>
+  </si>
+  <si>
+    <t>J. Erving (17.6)</t>
+  </si>
+  <si>
+    <t>S. Nater</t>
+  </si>
+  <si>
+    <t>J. Erving (2299)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (1538)</t>
+  </si>
+  <si>
+    <t>A. Smith (619)</t>
+  </si>
+  <si>
+    <t>J. Erving (16.5)</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>B. Cunningham</t>
+  </si>
+  <si>
+    <t>B. Taylor</t>
+  </si>
+  <si>
+    <t>D. Issel (2292)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (1476)</t>
+  </si>
+  <si>
+    <t>C. Williams (582)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (18.5)</t>
+  </si>
+  <si>
+    <t>A. Gilmore</t>
+  </si>
+  <si>
+    <t>D. Issel (2538)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (1491)</t>
+  </si>
+  <si>
+    <t>B. Melchionni (669)</t>
+  </si>
+  <si>
+    <t>A. Gilmore (19.8)</t>
+  </si>
+  <si>
+    <t>1970-71</t>
+  </si>
+  <si>
+    <t>Milwaukee Bucks</t>
+  </si>
+  <si>
+    <t>K. Abdul-Jabbar (2596)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1493)</t>
+  </si>
+  <si>
+    <t>N. Van Lier (832)</t>
+  </si>
+  <si>
+    <t>K. Abdul-Jabbar (22.3)</t>
+  </si>
+  <si>
+    <t>Utah Stars</t>
+  </si>
+  <si>
+    <t>M. Daniels</t>
+  </si>
+  <si>
+    <t>D. Issel (2480)</t>
+  </si>
+  <si>
+    <t>M. Daniels (1475)</t>
+  </si>
+  <si>
+    <t>B. Melchionni (672)</t>
+  </si>
+  <si>
+    <t>Z. Beaty (16.0)</t>
+  </si>
+  <si>
+    <t>1969-70</t>
+  </si>
+  <si>
+    <t>W. Reed</t>
+  </si>
+  <si>
+    <t>K. Abdul-Jabbar (2361)</t>
+  </si>
+  <si>
+    <t>E. Hayes (1386)</t>
+  </si>
+  <si>
+    <t>L. Wilkens (683)</t>
+  </si>
+  <si>
+    <t>J. West (15.2)</t>
+  </si>
+  <si>
+    <t>S. Haywood</t>
+  </si>
+  <si>
+    <t>S. Haywood (2519)</t>
+  </si>
+  <si>
+    <t>S. Haywood (1637)</t>
+  </si>
+  <si>
+    <t>L. Brown (580)</t>
+  </si>
+  <si>
+    <t>S. Haywood (17.1)</t>
+  </si>
+  <si>
+    <t>1968-69</t>
+  </si>
+  <si>
+    <t>W. Unseld</t>
+  </si>
+  <si>
+    <t>E. Hayes (2327)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1712)</t>
+  </si>
+  <si>
+    <t>O. Robertson (772)</t>
+  </si>
+  <si>
+    <t>W. Reed (14.7)</t>
+  </si>
+  <si>
+    <t>Oakland Oaks</t>
+  </si>
+  <si>
+    <t>W. Jabali</t>
+  </si>
+  <si>
+    <t>L. Jones (2133)</t>
+  </si>
+  <si>
+    <t>M. Daniels (1256)</t>
+  </si>
+  <si>
+    <t>L. Brown (544)</t>
+  </si>
+  <si>
+    <t>J. Jones (16.1)</t>
+  </si>
+  <si>
+    <t>1967-68</t>
+  </si>
+  <si>
+    <t>W. Chamberlain</t>
+  </si>
+  <si>
+    <t>E. Monroe</t>
+  </si>
+  <si>
+    <t>D. Bing (2142)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1952)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (702)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (20.4)</t>
+  </si>
+  <si>
+    <t>Pittsburgh Pipers</t>
+  </si>
+  <si>
+    <t>C. Hawkins</t>
+  </si>
+  <si>
+    <t>D. Moe (1884)</t>
+  </si>
+  <si>
+    <t>M. Daniels (1213)</t>
+  </si>
+  <si>
+    <t>L. Brown (506)</t>
+  </si>
+  <si>
+    <t>C. Hawkins (17.9)</t>
+  </si>
+  <si>
+    <t>1966-67</t>
+  </si>
+  <si>
+    <t>D. Bing</t>
+  </si>
+  <si>
+    <t>R. Barry (2775)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1957)</t>
+  </si>
+  <si>
+    <t>G. Rodgers (908)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (21.9)</t>
+  </si>
+  <si>
+    <t>1965-66</t>
+  </si>
+  <si>
+    <t>R. Barry</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2649)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1943)</t>
+  </si>
+  <si>
+    <t>O. Robertson (847)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (21.4)</t>
+  </si>
+  <si>
+    <t>1964-65</t>
+  </si>
+  <si>
+    <t>B. Russell</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2534)</t>
+  </si>
+  <si>
+    <t>B. Russell (1878)</t>
+  </si>
+  <si>
+    <t>O. Robertson (861)</t>
+  </si>
+  <si>
+    <t>O. Robertson (17.0)</t>
+  </si>
+  <si>
+    <t>1963-64</t>
+  </si>
+  <si>
+    <t>O. Robertson</t>
+  </si>
+  <si>
+    <t>J. Lucas</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2948)</t>
+  </si>
+  <si>
+    <t>B. Russell (1930)</t>
+  </si>
+  <si>
+    <t>O. Robertson (868)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (25.0)</t>
+  </si>
+  <si>
+    <t>1962-63</t>
+  </si>
+  <si>
+    <t>T. Dischinger</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (3586)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1946)</t>
+  </si>
+  <si>
+    <t>G. Rodgers (825)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (20.9)</t>
+  </si>
+  <si>
+    <t>1961-62</t>
+  </si>
+  <si>
+    <t>W. Bellamy</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (4029)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2052)</t>
+  </si>
+  <si>
+    <t>O. Robertson (899)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (23.1)</t>
+  </si>
+  <si>
+    <t>1960-61</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (3033)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2149)</t>
+  </si>
+  <si>
+    <t>O. Robertson (690)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (18.8)</t>
+  </si>
+  <si>
+    <t>1959-60</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (2707)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (1941)</t>
+  </si>
+  <si>
+    <t>B. Cousy (715)</t>
+  </si>
+  <si>
+    <t>W. Chamberlain (17.0)</t>
+  </si>
+  <si>
+    <t>1958-59</t>
+  </si>
+  <si>
+    <t>B. Pettit</t>
+  </si>
+  <si>
+    <t>E. Baylor</t>
+  </si>
+  <si>
+    <t>B. Pettit (2105)</t>
+  </si>
+  <si>
+    <t>B. Russell (1612)</t>
+  </si>
+  <si>
+    <t>B. Cousy (557)</t>
+  </si>
+  <si>
+    <t>B. Pettit (14.8)</t>
+  </si>
+  <si>
+    <t>1957-58</t>
+  </si>
+  <si>
+    <t>St. Louis Hawks</t>
+  </si>
+  <si>
+    <t>W. Sauldsberry</t>
+  </si>
+  <si>
+    <t>G. Yardley (2001)</t>
+  </si>
+  <si>
+    <t>B. Russell (1564)</t>
+  </si>
+  <si>
+    <t>B. Cousy (463)</t>
+  </si>
+  <si>
+    <t>D. Schayes (13.7)</t>
+  </si>
+  <si>
+    <t>1956-57</t>
+  </si>
+  <si>
+    <t>B. Cousy</t>
+  </si>
+  <si>
+    <t>T. Heinsohn</t>
+  </si>
+  <si>
+    <t>P. Arizin (1817)</t>
+  </si>
+  <si>
+    <t>M. Stokes (1256)</t>
+  </si>
+  <si>
+    <t>B. Cousy (478)</t>
+  </si>
+  <si>
+    <t>N. Johnston (13.7)</t>
+  </si>
+  <si>
+    <t>1955-56</t>
+  </si>
+  <si>
+    <t>Philadelphia Warriors</t>
+  </si>
+  <si>
+    <t>M. Stokes</t>
+  </si>
+  <si>
+    <t>B. Pettit (1849)</t>
+  </si>
+  <si>
+    <t>B. Pettit (1164)</t>
+  </si>
+  <si>
+    <t>B. Cousy (642)</t>
+  </si>
+  <si>
+    <t>N. Johnston (13.9)</t>
+  </si>
+  <si>
+    <t>1954-55</t>
+  </si>
+  <si>
+    <t>Syracuse Nationals</t>
+  </si>
+  <si>
+    <t>N. Johnston (1631)</t>
+  </si>
+  <si>
+    <t>N. Johnston (1085)</t>
+  </si>
+  <si>
+    <t>N. Johnston (15.4)</t>
+  </si>
+  <si>
+    <t>1953-54</t>
+  </si>
+  <si>
+    <t>Minneapolis Lakers</t>
+  </si>
+  <si>
+    <t>R. Felix</t>
+  </si>
+  <si>
+    <t>N. Johnston (1759)</t>
+  </si>
+  <si>
+    <t>H. Gallatin (1098)</t>
+  </si>
+  <si>
+    <t>B. Cousy (518)</t>
+  </si>
+  <si>
+    <t>N. Johnston (18.3)</t>
+  </si>
+  <si>
+    <t>1952-53</t>
+  </si>
+  <si>
+    <t>M. Meineke</t>
+  </si>
+  <si>
+    <t>N. Johnston (1564)</t>
+  </si>
+  <si>
+    <t>G. Mikan (1007)</t>
+  </si>
+  <si>
+    <t>B. Cousy (547)</t>
+  </si>
+  <si>
+    <t>N. Johnston (15.3)</t>
+  </si>
+  <si>
+    <t>1951-52</t>
+  </si>
+  <si>
+    <t>P. Arizin (1674)</t>
+  </si>
+  <si>
+    <t>L. Foust (880)</t>
+  </si>
+  <si>
+    <t>A. Phillip (539)</t>
+  </si>
+  <si>
+    <t>P. Arizin (16.0)</t>
+  </si>
+  <si>
+    <t>1950-51</t>
+  </si>
+  <si>
+    <t>Rochester Royals</t>
+  </si>
+  <si>
+    <t>P. Arizin</t>
+  </si>
+  <si>
+    <t>G. Mikan (1932)</t>
+  </si>
+  <si>
+    <t>D. Schayes (1080)</t>
+  </si>
+  <si>
+    <t>A. Phillip (414)</t>
+  </si>
+  <si>
+    <t>G. Mikan (23.4)</t>
+  </si>
+  <si>
+    <t>1949-50</t>
+  </si>
+  <si>
+    <t>A. Groza</t>
+  </si>
+  <si>
+    <t>G. Mikan (1865)</t>
+  </si>
+  <si>
+    <t>D. McGuire (386)</t>
+  </si>
+  <si>
+    <t>G. Mikan (21.1)</t>
+  </si>
+  <si>
+    <t>1948-49</t>
+  </si>
+  <si>
+    <t>BAA</t>
+  </si>
+  <si>
+    <t>H. Shannon</t>
+  </si>
+  <si>
+    <t>G. Mikan (1698)</t>
+  </si>
+  <si>
+    <t>B. Davies (321)</t>
+  </si>
+  <si>
+    <t>G. Mikan (20.9)</t>
+  </si>
+  <si>
+    <t>1947-48</t>
+  </si>
+  <si>
+    <t>Baltimore Bullets</t>
+  </si>
+  <si>
+    <t>P. Hoffman</t>
+  </si>
+  <si>
+    <t>M. Zaslofsky (1007)</t>
+  </si>
+  <si>
+    <t>H. Dallmar (120)</t>
+  </si>
+  <si>
+    <t>B. Feerick (10.5)</t>
+  </si>
+  <si>
+    <t>1946-47</t>
+  </si>
+  <si>
+    <t>J. Fulks (1389)</t>
+  </si>
+  <si>
+    <t>E. Calverley (202)</t>
+  </si>
+  <si>
+    <t>B. Feerick (18.6)</t>
+  </si>
+  <si>
+    <t>J. Erving, G. McGinnis</t>
+  </si>
+  <si>
+    <t>D. Cowens, G. Petrie</t>
+  </si>
+  <si>
+    <t>D. Issel, C. Scott</t>
+  </si>
+  <si>
+    <t>M. Hutchins, B. Tosheff</t>
   </si>
 </sst>
 </file>
@@ -1097,9 +1703,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1414,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F94185-40E2-48D3-B637-1DF5A1216488}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:XFD50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,14 +2036,9 @@
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1466,86 +2066,63 @@
       <c r="I1" t="s">
         <v>322</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>323</v>
       </c>
-      <c r="K1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" t="s">
         <v>324</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="F2" t="s">
         <v>325</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="G2" t="s">
         <v>326</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="H2" t="s">
         <v>327</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="I2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>329</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>330</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
         <v>331</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
         <v>332</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F3" t="s">
         <v>333</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
         <v>334</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H3" t="s">
         <v>335</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="I3" t="s">
         <v>336</v>
       </c>
-      <c r="D3" t="s">
-        <v>337</v>
-      </c>
-      <c r="E3" t="s">
-        <v>338</v>
-      </c>
-      <c r="F3" t="s">
-        <v>339</v>
-      </c>
-      <c r="G3" t="s">
-        <v>340</v>
-      </c>
-      <c r="H3" t="s">
-        <v>341</v>
-      </c>
-      <c r="I3" t="s">
-        <v>342</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1574,7 +2151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +2180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1632,7 +2209,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1661,7 +2238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1690,7 +2267,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1719,7 +2296,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1748,7 +2325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1777,7 +2354,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1806,7 +2383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -1835,7 +2412,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -1864,7 +2441,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -1893,7 +2470,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -2794,118 +3371,1062 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>337</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
       <c r="D47" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
       <c r="E47" t="s">
-        <v>292</v>
+        <v>339</v>
       </c>
       <c r="F47" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
       <c r="G47" t="s">
-        <v>294</v>
+        <v>341</v>
       </c>
       <c r="H47" t="s">
-        <v>295</v>
+        <v>342</v>
       </c>
       <c r="I47" t="s">
-        <v>296</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>257</v>
+        <v>291</v>
       </c>
       <c r="E48" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F48" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="G48" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="H48" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I48" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>337</v>
       </c>
       <c r="C49" t="s">
-        <v>304</v>
+        <v>344</v>
       </c>
       <c r="D49" t="s">
-        <v>305</v>
+        <v>541</v>
       </c>
       <c r="E49" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="F49" t="s">
-        <v>306</v>
+        <v>346</v>
       </c>
       <c r="G49" t="s">
-        <v>307</v>
+        <v>347</v>
       </c>
       <c r="H49" t="s">
-        <v>308</v>
+        <v>348</v>
       </c>
       <c r="I49" t="s">
-        <v>309</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
         <v>257</v>
       </c>
       <c r="E50" t="s">
+        <v>298</v>
+      </c>
+      <c r="F50" t="s">
+        <v>299</v>
+      </c>
+      <c r="G50" t="s">
+        <v>300</v>
+      </c>
+      <c r="H50" t="s">
+        <v>301</v>
+      </c>
+      <c r="I50" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>297</v>
+      </c>
+      <c r="B51" t="s">
+        <v>337</v>
+      </c>
+      <c r="C51" t="s">
+        <v>338</v>
+      </c>
+      <c r="D51" t="s">
+        <v>250</v>
+      </c>
+      <c r="E51" t="s">
+        <v>350</v>
+      </c>
+      <c r="F51" t="s">
+        <v>351</v>
+      </c>
+      <c r="G51" t="s">
+        <v>352</v>
+      </c>
+      <c r="H51" t="s">
+        <v>353</v>
+      </c>
+      <c r="I51" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>303</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>304</v>
+      </c>
+      <c r="D52" t="s">
+        <v>305</v>
+      </c>
+      <c r="E52" t="s">
+        <v>291</v>
+      </c>
+      <c r="F52" t="s">
+        <v>306</v>
+      </c>
+      <c r="G52" t="s">
+        <v>307</v>
+      </c>
+      <c r="H52" t="s">
+        <v>308</v>
+      </c>
+      <c r="I52" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>303</v>
+      </c>
+      <c r="B53" t="s">
+        <v>337</v>
+      </c>
+      <c r="C53" t="s">
+        <v>355</v>
+      </c>
+      <c r="D53" t="s">
+        <v>356</v>
+      </c>
+      <c r="E53" t="s">
+        <v>357</v>
+      </c>
+      <c r="F53" t="s">
+        <v>358</v>
+      </c>
+      <c r="G53" t="s">
+        <v>359</v>
+      </c>
+      <c r="H53" t="s">
+        <v>360</v>
+      </c>
+      <c r="I53" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>310</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" t="s">
         <v>311</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F54" t="s">
         <v>312</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G54" t="s">
         <v>313</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H54" t="s">
         <v>314</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I54" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>310</v>
+      </c>
+      <c r="B55" t="s">
+        <v>337</v>
+      </c>
+      <c r="C55" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" t="s">
+        <v>362</v>
+      </c>
+      <c r="E55" t="s">
+        <v>362</v>
+      </c>
+      <c r="F55" t="s">
+        <v>363</v>
+      </c>
+      <c r="G55" t="s">
+        <v>364</v>
+      </c>
+      <c r="H55" t="s">
+        <v>365</v>
+      </c>
+      <c r="I55" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>367</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>368</v>
+      </c>
+      <c r="D56" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" t="s">
+        <v>542</v>
+      </c>
+      <c r="F56" t="s">
+        <v>369</v>
+      </c>
+      <c r="G56" t="s">
+        <v>370</v>
+      </c>
+      <c r="H56" t="s">
+        <v>371</v>
+      </c>
+      <c r="I56" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>367</v>
+      </c>
+      <c r="B57" t="s">
+        <v>337</v>
+      </c>
+      <c r="C57" t="s">
+        <v>373</v>
+      </c>
+      <c r="D57" t="s">
+        <v>374</v>
+      </c>
+      <c r="E57" t="s">
+        <v>543</v>
+      </c>
+      <c r="F57" t="s">
+        <v>375</v>
+      </c>
+      <c r="G57" t="s">
+        <v>376</v>
+      </c>
+      <c r="H57" t="s">
+        <v>377</v>
+      </c>
+      <c r="I57" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>379</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>304</v>
+      </c>
+      <c r="D58" t="s">
+        <v>380</v>
+      </c>
+      <c r="E58" t="s">
+        <v>257</v>
+      </c>
+      <c r="F58" t="s">
+        <v>381</v>
+      </c>
+      <c r="G58" t="s">
+        <v>382</v>
+      </c>
+      <c r="H58" t="s">
+        <v>383</v>
+      </c>
+      <c r="I58" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>379</v>
+      </c>
+      <c r="B59" t="s">
+        <v>337</v>
+      </c>
+      <c r="C59" t="s">
+        <v>355</v>
+      </c>
+      <c r="D59" t="s">
+        <v>385</v>
+      </c>
+      <c r="E59" t="s">
+        <v>385</v>
+      </c>
+      <c r="F59" t="s">
+        <v>386</v>
+      </c>
+      <c r="G59" t="s">
+        <v>387</v>
+      </c>
+      <c r="H59" t="s">
+        <v>388</v>
+      </c>
+      <c r="I59" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>390</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" t="s">
+        <v>391</v>
+      </c>
+      <c r="E60" t="s">
+        <v>391</v>
+      </c>
+      <c r="F60" t="s">
+        <v>392</v>
+      </c>
+      <c r="G60" t="s">
+        <v>393</v>
+      </c>
+      <c r="H60" t="s">
+        <v>394</v>
+      </c>
+      <c r="I60" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>390</v>
+      </c>
+      <c r="B61" t="s">
+        <v>337</v>
+      </c>
+      <c r="C61" t="s">
+        <v>396</v>
+      </c>
+      <c r="D61" t="s">
+        <v>374</v>
+      </c>
+      <c r="E61" t="s">
+        <v>397</v>
+      </c>
+      <c r="F61" t="s">
+        <v>398</v>
+      </c>
+      <c r="G61" t="s">
+        <v>399</v>
+      </c>
+      <c r="H61" t="s">
+        <v>400</v>
+      </c>
+      <c r="I61" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>402</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" t="s">
+        <v>403</v>
+      </c>
+      <c r="E62" t="s">
+        <v>404</v>
+      </c>
+      <c r="F62" t="s">
+        <v>405</v>
+      </c>
+      <c r="G62" t="s">
+        <v>406</v>
+      </c>
+      <c r="H62" t="s">
+        <v>407</v>
+      </c>
+      <c r="I62" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>402</v>
+      </c>
+      <c r="B63" t="s">
+        <v>337</v>
+      </c>
+      <c r="C63" t="s">
+        <v>409</v>
+      </c>
+      <c r="D63" t="s">
+        <v>410</v>
+      </c>
+      <c r="E63" t="s">
+        <v>374</v>
+      </c>
+      <c r="F63" t="s">
+        <v>411</v>
+      </c>
+      <c r="G63" t="s">
+        <v>412</v>
+      </c>
+      <c r="H63" t="s">
+        <v>413</v>
+      </c>
+      <c r="I63" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>415</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>236</v>
+      </c>
+      <c r="D64" t="s">
+        <v>403</v>
+      </c>
+      <c r="E64" t="s">
+        <v>416</v>
+      </c>
+      <c r="F64" t="s">
+        <v>417</v>
+      </c>
+      <c r="G64" t="s">
+        <v>418</v>
+      </c>
+      <c r="H64" t="s">
+        <v>419</v>
+      </c>
+      <c r="I64" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>421</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" t="s">
+        <v>403</v>
+      </c>
+      <c r="E65" t="s">
+        <v>422</v>
+      </c>
+      <c r="F65" t="s">
+        <v>423</v>
+      </c>
+      <c r="G65" t="s">
+        <v>424</v>
+      </c>
+      <c r="H65" t="s">
+        <v>425</v>
+      </c>
+      <c r="I65" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>427</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" t="s">
+        <v>428</v>
+      </c>
+      <c r="E66" t="s">
+        <v>380</v>
+      </c>
+      <c r="F66" t="s">
+        <v>429</v>
+      </c>
+      <c r="G66" t="s">
+        <v>430</v>
+      </c>
+      <c r="H66" t="s">
+        <v>431</v>
+      </c>
+      <c r="I66" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>433</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" t="s">
+        <v>434</v>
+      </c>
+      <c r="E67" t="s">
+        <v>435</v>
+      </c>
+      <c r="F67" t="s">
+        <v>436</v>
+      </c>
+      <c r="G67" t="s">
+        <v>437</v>
+      </c>
+      <c r="H67" t="s">
+        <v>438</v>
+      </c>
+      <c r="I67" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>440</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" t="s">
+        <v>428</v>
+      </c>
+      <c r="E68" t="s">
+        <v>441</v>
+      </c>
+      <c r="F68" t="s">
+        <v>442</v>
+      </c>
+      <c r="G68" t="s">
+        <v>443</v>
+      </c>
+      <c r="H68" t="s">
+        <v>444</v>
+      </c>
+      <c r="I68" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>446</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>77</v>
+      </c>
+      <c r="D69" t="s">
+        <v>428</v>
+      </c>
+      <c r="E69" t="s">
+        <v>447</v>
+      </c>
+      <c r="F69" t="s">
+        <v>448</v>
+      </c>
+      <c r="G69" t="s">
+        <v>449</v>
+      </c>
+      <c r="H69" t="s">
+        <v>450</v>
+      </c>
+      <c r="I69" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>452</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" t="s">
+        <v>428</v>
+      </c>
+      <c r="E70" t="s">
+        <v>434</v>
+      </c>
+      <c r="F70" t="s">
+        <v>453</v>
+      </c>
+      <c r="G70" t="s">
+        <v>454</v>
+      </c>
+      <c r="H70" t="s">
+        <v>455</v>
+      </c>
+      <c r="I70" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>457</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>77</v>
+      </c>
+      <c r="D71" t="s">
+        <v>403</v>
+      </c>
+      <c r="E71" t="s">
+        <v>403</v>
+      </c>
+      <c r="F71" t="s">
+        <v>458</v>
+      </c>
+      <c r="G71" t="s">
+        <v>459</v>
+      </c>
+      <c r="H71" t="s">
+        <v>460</v>
+      </c>
+      <c r="I71" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>462</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>77</v>
+      </c>
+      <c r="D72" t="s">
+        <v>463</v>
+      </c>
+      <c r="E72" t="s">
+        <v>464</v>
+      </c>
+      <c r="F72" t="s">
+        <v>465</v>
+      </c>
+      <c r="G72" t="s">
+        <v>466</v>
+      </c>
+      <c r="H72" t="s">
+        <v>467</v>
+      </c>
+      <c r="I72" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>469</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" t="s">
+        <v>470</v>
+      </c>
+      <c r="D73" t="s">
+        <v>428</v>
+      </c>
+      <c r="E73" t="s">
+        <v>471</v>
+      </c>
+      <c r="F73" t="s">
+        <v>472</v>
+      </c>
+      <c r="G73" t="s">
+        <v>473</v>
+      </c>
+      <c r="H73" t="s">
+        <v>474</v>
+      </c>
+      <c r="I73" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>476</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" t="s">
+        <v>477</v>
+      </c>
+      <c r="E74" t="s">
+        <v>478</v>
+      </c>
+      <c r="F74" t="s">
+        <v>479</v>
+      </c>
+      <c r="G74" t="s">
+        <v>480</v>
+      </c>
+      <c r="H74" t="s">
+        <v>481</v>
+      </c>
+      <c r="I74" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>483</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" t="s">
+        <v>484</v>
+      </c>
+      <c r="D75" t="s">
+        <v>463</v>
+      </c>
+      <c r="E75" t="s">
+        <v>485</v>
+      </c>
+      <c r="F75" t="s">
+        <v>486</v>
+      </c>
+      <c r="G75" t="s">
+        <v>487</v>
+      </c>
+      <c r="H75" t="s">
+        <v>488</v>
+      </c>
+      <c r="I75" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>490</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>491</v>
+      </c>
+      <c r="E76" t="s">
+        <v>463</v>
+      </c>
+      <c r="F76" t="s">
+        <v>492</v>
+      </c>
+      <c r="G76" t="s">
+        <v>493</v>
+      </c>
+      <c r="H76" t="s">
+        <v>467</v>
+      </c>
+      <c r="I76" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>495</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>496</v>
+      </c>
+      <c r="E77" t="s">
+        <v>497</v>
+      </c>
+      <c r="F77" t="s">
+        <v>498</v>
+      </c>
+      <c r="G77" t="s">
+        <v>499</v>
+      </c>
+      <c r="H77" t="s">
+        <v>500</v>
+      </c>
+      <c r="I77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>502</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s">
+        <v>496</v>
+      </c>
+      <c r="E78" t="s">
+        <v>503</v>
+      </c>
+      <c r="F78" t="s">
+        <v>504</v>
+      </c>
+      <c r="G78" t="s">
+        <v>505</v>
+      </c>
+      <c r="H78" t="s">
+        <v>506</v>
+      </c>
+      <c r="I78" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>508</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" t="s">
+        <v>496</v>
+      </c>
+      <c r="E79" t="s">
+        <v>544</v>
+      </c>
+      <c r="F79" t="s">
+        <v>509</v>
+      </c>
+      <c r="G79" t="s">
+        <v>510</v>
+      </c>
+      <c r="H79" t="s">
+        <v>511</v>
+      </c>
+      <c r="I79" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>513</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" t="s">
+        <v>514</v>
+      </c>
+      <c r="E80" t="s">
+        <v>515</v>
+      </c>
+      <c r="F80" t="s">
+        <v>516</v>
+      </c>
+      <c r="G80" t="s">
+        <v>517</v>
+      </c>
+      <c r="H80" t="s">
+        <v>518</v>
+      </c>
+      <c r="I80" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>520</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>496</v>
+      </c>
+      <c r="E81" t="s">
+        <v>521</v>
+      </c>
+      <c r="F81" t="s">
+        <v>522</v>
+      </c>
+      <c r="H81" t="s">
+        <v>523</v>
+      </c>
+      <c r="I81" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>525</v>
+      </c>
+      <c r="B82" t="s">
+        <v>526</v>
+      </c>
+      <c r="C82" t="s">
+        <v>496</v>
+      </c>
+      <c r="E82" t="s">
+        <v>527</v>
+      </c>
+      <c r="F82" t="s">
+        <v>528</v>
+      </c>
+      <c r="H82" t="s">
+        <v>529</v>
+      </c>
+      <c r="I82" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>531</v>
+      </c>
+      <c r="B83" t="s">
+        <v>526</v>
+      </c>
+      <c r="C83" t="s">
+        <v>532</v>
+      </c>
+      <c r="E83" t="s">
+        <v>533</v>
+      </c>
+      <c r="F83" t="s">
+        <v>534</v>
+      </c>
+      <c r="H83" t="s">
+        <v>535</v>
+      </c>
+      <c r="I83" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>537</v>
+      </c>
+      <c r="B84" t="s">
+        <v>526</v>
+      </c>
+      <c r="C84" t="s">
+        <v>484</v>
+      </c>
+      <c r="F84" t="s">
+        <v>538</v>
+      </c>
+      <c r="H84" t="s">
+        <v>539</v>
+      </c>
+      <c r="I84" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>